<commit_message>
Added letters to figure 4
</commit_message>
<xml_diff>
--- a/Outputs/YII_Emm_Pairwise.xlsx
+++ b/Outputs/YII_Emm_Pairwise.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pachacuti/Documents/Projects/environmental-cofactors/4.IPAM/Outputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pachacuti/Documents/Projects/environmental-cofactors/3.IPAM/Outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4918B8B1-1B63-3643-A78D-29D5C1A7774D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A916CD-6D10-6243-8870-F19CB158FB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="880" windowWidth="28040" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="840" windowWidth="28040" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="YIIAcerEmm" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Nutrients</t>
   </si>
@@ -134,6 +147,12 @@
   </si>
   <si>
     <t xml:space="preserve">      But we also did not show them to be the same.</t>
+  </si>
+  <si>
+    <t>28 vs 31</t>
+  </si>
+  <si>
+    <t>H vs L</t>
   </si>
 </sst>
 </file>
@@ -639,7 +658,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -682,8 +701,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -708,8 +728,10 @@
     <xf numFmtId="1" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="21" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -749,6 +771,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -1063,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1087,15 +1110,16 @@
     <col min="14" max="14" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="8.5" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="1"/>
+    <col min="18" max="18" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -1142,8 +1166,14 @@
       <c r="Q3" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R3" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1192,8 +1222,20 @@
       <c r="Q4" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R4" s="25">
+        <f>(L4-L6)/L6</f>
+        <v>-2.4244072419990593E-2</v>
+      </c>
+      <c r="S4" s="25">
+        <f>(O6-O4)/O4</f>
+        <v>2.7532753895653933E-2</v>
+      </c>
+      <c r="T4" s="25">
+        <f>(L5-L4)/L4</f>
+        <v>9.2201518027521714E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
@@ -1242,8 +1284,17 @@
       <c r="Q5" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R5" s="25">
+        <f>(L5-L7)/L7</f>
+        <v>-2.4027902564687814E-2</v>
+      </c>
+      <c r="S5" s="25">
+        <f>(O7-O5)/O5</f>
+        <v>2.7287731676172901E-2</v>
+      </c>
+      <c r="T5" s="25"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>16</v>
       </c>
@@ -1290,8 +1341,12 @@
       <c r="Q6" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T6" s="25">
+        <f>(L7-L6)/L6</f>
+        <v>8.9966177747229405E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="J7" s="14" t="s">
         <v>5</v>
       </c>
@@ -1317,12 +1372,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="15"/>
       <c r="B9" s="16" t="s">
         <v>19</v>
@@ -1347,7 +1402,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
@@ -1374,7 +1429,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>27</v>
       </c>
@@ -1403,27 +1458,27 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="J12" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="J13" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="J14" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="J15" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="J16" s="1" t="s">
         <v>37</v>
       </c>

</xml_diff>